<commit_message>
set NM range 1.25-2.25
</commit_message>
<xml_diff>
--- a/atomoxetine/atomoxetine_Pre_and_Post_Test_Alerts_and_Flow_Chart.xlsx
+++ b/atomoxetine/atomoxetine_Pre_and_Post_Test_Alerts_and_Flow_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrin/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACCD670-C870-3849-B4D5-1B2180D0AC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B967DF0-4E19-924A-B5B1-F8F496EBC730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="460" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="2340" windowWidth="25440" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-and Post-Test Alerts" sheetId="21" r:id="rId1"/>
@@ -333,16 +333,23 @@
     <t>&gt;2.25</t>
   </si>
   <si>
-    <t>1.5-2.25</t>
+    <t>1.25-2.25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -529,74 +536,77 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2968,9 +2978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2999,12 +3007,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3028,7 +3036,7 @@
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -3045,7 +3053,7 @@
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="7" t="s">

</xml_diff>